<commit_message>
candidate v3.1 rel 1
</commit_message>
<xml_diff>
--- a/mark59-server-metrics/src/test/resources/simpleSheetWithLocalhostProfileForEachOs/mark59serverprofiles.xlsx
+++ b/mark59-server-metrics/src/test/resources/simpleSheetWithLocalhostProfileForEachOs/mark59serverprofiles.xlsx
@@ -1,30 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitrepo\mark-5-9\mark59-wip\mark59-server-metrics\src\test\resources\simpleSheetWithLocalhostProfileForEachOs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA23838-450C-4FF9-80A3-715A4ADFE7D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="SERVERPROFILES" sheetId="1" r:id="rId1"/>
-    <sheet name="SERVERCOMMANDLINKS" sheetId="2" r:id="rId2"/>
-    <sheet name="COMMANDS" sheetId="3" r:id="rId3"/>
-    <sheet name="COMMANDPARSERLINKS" sheetId="4" r:id="rId4"/>
-    <sheet name="COMMANDRESPONSEPARSERS" sheetId="5" r:id="rId5"/>
+    <sheet name="SERVERPROFILES" r:id="rId3" sheetId="1"/>
+    <sheet name="SERVERCOMMANDLINKS" r:id="rId4" sheetId="2"/>
+    <sheet name="COMMANDS" r:id="rId5" sheetId="3"/>
+    <sheet name="COMMANDPARSERLINKS" r:id="rId6" sheetId="4"/>
+    <sheet name="COMMANDRESPONSEPARSERS" r:id="rId7" sheetId="5"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="144">
   <si>
     <t>SERVER_PROFILE_NAME</t>
   </si>
@@ -165,9 +157,6 @@
   </si>
   <si>
     <t>WinServerName</t>
-  </si>
-  <si>
-    <t>xnr</t>
   </si>
   <si>
     <t>COMMAND_NAME</t>
@@ -743,28 +732,34 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
       <color indexed="9"/>
-      <name val="Calibri"/>
+      <b val="true"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="darkGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="16"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -786,379 +781,69 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="48.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="102.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="152.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="2" width="48.17578125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="17.41015625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="16.78515625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="22.79296875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="11.62109375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="11.74609375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="19.46484375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="19.5390625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="23.23828125" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="102.359375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="71.546875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s" s="1">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s" s="1">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s" s="1">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s" s="1">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s" s="1">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s" s="1">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s" s="1">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1193,7 +878,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1228,7 +913,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1263,7 +948,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1298,7 +983,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1333,7 +1018,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1368,13 +1053,20 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8">
       <c r="A8" t="s">
         <v>27</v>
       </c>
       <c r="B8" t="s">
         <v>28</v>
       </c>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
       <c r="J8" t="s">
         <v>29</v>
       </c>
@@ -1382,13 +1074,20 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9">
       <c r="A9" t="s">
         <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>28</v>
       </c>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
       <c r="J9" t="s">
         <v>32</v>
       </c>
@@ -1396,7 +1095,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1431,7 +1130,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -1466,7 +1165,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -1501,7 +1200,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -1536,7 +1235,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -1571,7 +1270,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -1607,1050 +1306,1042 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="48.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.17578125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="43.234375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1" t="s" s="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" t="s">
         <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" t="s">
         <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" t="s">
         <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" t="s">
         <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" t="s">
         <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" t="s">
         <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" t="s">
         <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12">
       <c r="A12" t="s">
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13">
       <c r="A13" t="s">
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14">
       <c r="A14" t="s">
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15">
       <c r="A15" t="s">
         <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16">
       <c r="A16" t="s">
         <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17">
       <c r="A17" t="s">
         <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18">
       <c r="A18" t="s">
         <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19">
       <c r="A19" t="s">
         <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20">
       <c r="A20" t="s">
         <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21">
       <c r="A21" t="s">
         <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22">
       <c r="A22" t="s">
         <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23">
       <c r="A23" t="s">
         <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24">
       <c r="A24" t="s">
         <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="43.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="223.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="117.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="62.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.234375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="17.41015625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="223.87109375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="16.45703125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="117.37890625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="62.10546875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s" s="1">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s" s="1">
         <v>64</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" t="s" s="1">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s" s="1">
         <v>65</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
         <v>23</v>
       </c>
       <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
         <v>67</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>68</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>69</v>
       </c>
-      <c r="F2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
       <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
         <v>71</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>72</v>
       </c>
-      <c r="E3" t="s">
-        <v>73</v>
-      </c>
       <c r="F3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
       </c>
       <c r="C5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" t="s">
         <v>75</v>
       </c>
-      <c r="D5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5" t="s">
-        <v>76</v>
-      </c>
       <c r="F5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" t="s">
         <v>78</v>
       </c>
-      <c r="D7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E7" t="s">
-        <v>79</v>
-      </c>
       <c r="F7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
       <c r="C10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" t="s">
         <v>82</v>
       </c>
-      <c r="D10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E10" t="s">
-        <v>83</v>
-      </c>
       <c r="F10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
         <v>28</v>
       </c>
       <c r="C12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" t="s">
         <v>85</v>
       </c>
-      <c r="D12" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>86</v>
       </c>
-      <c r="F12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
         <v>28</v>
       </c>
       <c r="C13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" t="s">
         <v>88</v>
       </c>
-      <c r="D13" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>89</v>
       </c>
-      <c r="F13" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
       </c>
       <c r="C14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
         <v>91</v>
-      </c>
-      <c r="D14" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>92</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E15" t="s">
         <v>14</v>
       </c>
       <c r="F15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E16" t="s">
         <v>14</v>
       </c>
       <c r="F16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" t="s">
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E17" t="s">
         <v>14</v>
       </c>
       <c r="F17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="43.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.234375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="33.62109375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="4">
+      <c r="A4" t="s">
         <v>52</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="9">
+      <c r="A9" t="s">
         <v>59</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="10">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
         <v>60</v>
       </c>
-      <c r="B9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="B21" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>92</v>
-      </c>
-      <c r="B17" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>92</v>
-      </c>
-      <c r="B18" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>92</v>
-      </c>
-      <c r="B19" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" t="s">
-        <v>106</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="140.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="139.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="92.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.62109375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="18.55078125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="22.39453125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="140.3984375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="139.76953125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="92.921875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>94</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>106</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>107</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>108</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s" s="1">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" t="s">
+        <v>127</v>
+      </c>
+      <c r="E7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E8" t="s">
+        <v>128</v>
+      </c>
+      <c r="F8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="B9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>132</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D3" t="s">
-        <v>116</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C4" t="s">
-        <v>118</v>
-      </c>
-      <c r="D4" t="s">
-        <v>119</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D5" t="s">
-        <v>121</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C6" t="s">
-        <v>123</v>
-      </c>
-      <c r="D6" t="s">
-        <v>121</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="C10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" t="s">
+        <v>137</v>
+      </c>
+      <c r="D11" t="s">
+        <v>138</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" t="s">
+        <v>139</v>
+      </c>
+      <c r="D12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" t="s">
         <v>125</v>
       </c>
-      <c r="B7" t="s">
-        <v>126</v>
-      </c>
-      <c r="C7" t="s">
-        <v>127</v>
-      </c>
-      <c r="D7" t="s">
-        <v>128</v>
-      </c>
-      <c r="E7" t="s">
-        <v>129</v>
-      </c>
-      <c r="F7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>102</v>
-      </c>
-      <c r="B8" t="s">
-        <v>126</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" t="s">
-        <v>131</v>
-      </c>
-      <c r="E8" t="s">
-        <v>129</v>
-      </c>
-      <c r="F8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>96</v>
-      </c>
-      <c r="B9" t="s">
-        <v>132</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s">
-        <v>133</v>
-      </c>
-      <c r="E9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>103</v>
-      </c>
-      <c r="B10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C10" t="s">
-        <v>135</v>
-      </c>
-      <c r="D10" t="s">
-        <v>136</v>
-      </c>
-      <c r="E10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>104</v>
-      </c>
-      <c r="B11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C11" t="s">
-        <v>138</v>
-      </c>
-      <c r="D11" t="s">
-        <v>139</v>
-      </c>
-      <c r="E11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>105</v>
-      </c>
-      <c r="B12" t="s">
-        <v>111</v>
-      </c>
-      <c r="C12" t="s">
-        <v>140</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
         <v>141</v>
       </c>
-      <c r="E12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>106</v>
-      </c>
-      <c r="B13" t="s">
-        <v>126</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>142</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>143</v>
       </c>
-      <c r="F13" t="s">
-        <v>144</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>